<commit_message>
TST: no person itself in coauthor
</commit_message>
<xml_diff>
--- a/tests/outputs/recent-collabs/scopatz_doe.xlsx
+++ b/tests/outputs/recent-collabs/scopatz_doe.xlsx
@@ -539,21 +539,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>Scopatz</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>Anthony</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>The University of South Carolina</t>
-        </is>
-      </c>
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="6" t="n"/>

</xml_diff>